<commit_message>
pdu配电修改 pdu配电详情bug修改 机房拓扑bug修改 --2025/5/22 jiangjinchi
</commit_message>
<xml_diff>
--- a/yudao-module-room/yudao-module-room-biz/src/main/resources/file/机柜绑定关系表.xlsx
+++ b/yudao-module-room/yudao-module-room-biz/src/main/resources/file/机柜绑定关系表.xlsx
@@ -156,7 +156,7 @@
     <t>{.boxAddra}</t>
   </si>
   <si>
-    <t>{.boxIndexa}</t>
+    <t>{.outletIda}</t>
   </si>
   <si>
     <t>{.busKeyb}</t>
@@ -165,7 +165,7 @@
     <t>{.boxAddrb}</t>
   </si>
   <si>
-    <t>{.boxIndexb}</t>
+    <t>{.outletIdb}</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1158,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
@@ -1309,7 +1309,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>

</xml_diff>